<commit_message>
project started day1 first commit
</commit_message>
<xml_diff>
--- a/QALegend/src/test/resources/ExcelData.xlsx
+++ b/QALegend/src/test/resources/ExcelData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\CRM\QALegend\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Title</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hellodesc</t>
   </si>
 </sst>
 </file>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -396,6 +402,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated script 2nd day
</commit_message>
<xml_diff>
--- a/QALegend/src/test/resources/ExcelData.xlsx
+++ b/QALegend/src/test/resources/ExcelData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Title</t>
   </si>
@@ -32,25 +32,19 @@
     <t>Description</t>
   </si>
   <si>
-    <t>StartDate</t>
-  </si>
-  <si>
-    <t>StartTime</t>
-  </si>
-  <si>
-    <t>EndDate</t>
-  </si>
-  <si>
-    <t>EndTime</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Hello</t>
   </si>
   <si>
     <t>Hellodesc</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>TestSample</t>
   </si>
 </sst>
 </file>
@@ -368,18 +362,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,27 +382,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="D2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>